<commit_message>
BCRA-27,25 - Questionnaire Template & Consent Page
Change-Id: Ibb2238f3017246f07b899e67cd2cf54861758e68
</commit_message>
<xml_diff>
--- a/data/questionnaires/version1/question.xlsx
+++ b/data/questionnaires/version1/question.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
   <si>
     <t>SELF_FIRST_PERIOD</t>
   </si>
@@ -189,9 +189,6 @@
     <t>CONSENT_DATA_COMMERCIAL</t>
   </si>
   <si>
-    <t>CONSENT_INFO_SHEET_2</t>
-  </si>
-  <si>
     <t>FAMILY_AFFECTED_GRANDMOTHER_MOTHERS_AGE</t>
   </si>
   <si>
@@ -223,9 +220,6 @@
   </si>
   <si>
     <t>I agree to receiving my breast cancer risk via letter.</t>
-  </si>
-  <si>
-    <t>I have read and understood the information sheet for this study.</t>
   </si>
   <si>
     <t>I am happy to be contacted about participation in future research.</t>
@@ -664,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +684,7 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -708,16 +702,16 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -728,7 +722,7 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -737,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -757,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -777,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -797,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -817,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -837,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -858,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -878,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -898,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -906,10 +900,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -918,504 +912,510 @@
         <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>70</v>
+        <v>2</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
       <c r="G13">
-        <v>2</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>130</v>
+      </c>
       <c r="G14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
         <v>10</v>
       </c>
-      <c r="F15">
+      <c r="F17" s="1">
         <v>130</v>
       </c>
-      <c r="G15">
-        <v>4</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>5</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17">
-        <v>6</v>
+      <c r="G17" s="1">
+        <v>7</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1">
-        <v>130</v>
-      </c>
-      <c r="G18" s="1">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>8</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1">
+        <v>130</v>
       </c>
       <c r="G19">
         <v>8</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1">
-        <v>130</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1">
+        <v>130</v>
       </c>
       <c r="G21">
         <v>9</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22">
         <v>10</v>
       </c>
-      <c r="F22" s="1">
-        <v>130</v>
-      </c>
-      <c r="G22">
-        <v>9</v>
-      </c>
       <c r="I22" s="4" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1">
+        <v>130</v>
       </c>
       <c r="G23">
         <v>10</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>10</v>
-      </c>
-      <c r="F24" s="1">
-        <v>130</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <v>130</v>
       </c>
       <c r="G25">
         <v>11</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
         <v>13</v>
       </c>
       <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26" s="1">
-        <v>10</v>
-      </c>
-      <c r="F26" s="1">
-        <v>130</v>
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
       </c>
       <c r="G26">
-        <v>11</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>96</v>
+        <v>12</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>5</v>
-      </c>
-      <c r="F27">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="G27">
         <v>12</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="J27" t="s">
+        <v>81</v>
+      </c>
+      <c r="K27" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>45</v>
       </c>
       <c r="G28">
         <v>12</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J28" t="s">
-        <v>83</v>
-      </c>
-      <c r="K28" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E29">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="G29">
         <v>12</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="G30">
         <v>12</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E31">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F31">
-        <v>45</v>
+        <v>300</v>
       </c>
       <c r="G31">
         <v>12</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E32">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="F32">
         <v>300</v>
@@ -1424,164 +1424,138 @@
         <v>12</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D33">
-        <v>7</v>
-      </c>
-      <c r="E33">
-        <v>30</v>
-      </c>
-      <c r="F33">
-        <v>300</v>
+        <v>8</v>
       </c>
       <c r="G33">
         <v>12</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="J33" t="s">
+        <v>83</v>
+      </c>
+      <c r="K33" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G34">
         <v>12</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J34" t="s">
-        <v>85</v>
-      </c>
-      <c r="K34" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D35">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G35">
         <v>12</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D36">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G36">
         <v>12</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
+      </c>
+      <c r="J36" t="s">
+        <v>85</v>
+      </c>
+      <c r="K36" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G37">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J37" t="s">
-        <v>87</v>
-      </c>
-      <c r="K37" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G38">
         <v>13</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39">
-        <v>2</v>
-      </c>
-      <c r="G39">
-        <v>13</v>
-      </c>
-      <c r="I39" s="3" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BCRA-28 - Your History Page
Change-Id: Ie0f8895f359d6b90fabcf48727bdbc4007190336
</commit_message>
<xml_diff>
--- a/data/questionnaires/version1/question.xlsx
+++ b/data/questionnaires/version1/question.xlsx
@@ -661,7 +661,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,10 +1337,10 @@
         <v>4</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G29">
         <v>12</v>

</xml_diff>

<commit_message>
Fix questions, fix diagram of database model in architecture doc
Change-Id: I7fec38abbc647835af0ec4fa6ac14d596073790e
</commit_message>
<xml_diff>
--- a/data/questionnaires/version1/question.xlsx
+++ b/data/questionnaires/version1/question.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="95">
   <si>
     <t>SELF_FIRST_PERIOD</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>A biopsy is when a small amount of tissue is removed or a larger amount of tissue is removed by cutting pieces from the breast\, or a lump is taken from the breast for further examination. A biopsy is the removal of tissue from the breast\, not the removal of fluid.</t>
+  </si>
+  <si>
+    <t>How old is this sister (or if this sister is not alive\, how old was she when she died)?</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>